<commit_message>
Add Item Category to import
</commit_message>
<xml_diff>
--- a/app/files/import.xlsx
+++ b/app/files/import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabian/Developer/worldskills-infrastructure-list/app/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4F9446-9734-1245-AA28-0D0348F6FD6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C25C739-7CF2-1E4D-B369-FB89A5C5DD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="35680" windowHeight="20060" xr2:uid="{5FBD6D1F-86F2-0545-B2A7-D0DA7AB544F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Description</t>
   </si>
@@ -65,9 +65,6 @@
     <t>PO Number</t>
   </si>
   <si>
-    <t>|</t>
-  </si>
-  <si>
     <t>Electricity</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Item subcategory</t>
+  </si>
+  <si>
+    <t>Item category</t>
   </si>
 </sst>
 </file>
@@ -175,9 +175,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,7 +215,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -321,7 +321,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,7 +463,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,15 +471,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{765ECE00-6669-2344-BEA6-CFFEE1B8FFFE}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" ht="41" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,43 +511,40 @@
         <v>21</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Unit column to import.xlsx template
</commit_message>
<xml_diff>
--- a/app/files/import.xlsx
+++ b/app/files/import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabian/Developer/worldskills-infrastructure-list/app/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C25C739-7CF2-1E4D-B369-FB89A5C5DD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40D0553-BECD-C648-81DD-C90C2CA376A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="35680" windowHeight="20060" xr2:uid="{5FBD6D1F-86F2-0545-B2A7-D0DA7AB544F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Description</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Item category</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{765ECE00-6669-2344-BEA6-CFFEE1B8FFFE}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -479,7 +482,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="41" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,45 +508,48 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>